<commit_message>
tp with sa alg.
</commit_message>
<xml_diff>
--- a/Documentazione/excel/calcolo_perc.xlsx
+++ b/Documentazione/excel/calcolo_perc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Desktop\SUPSI\terza\2semestre\algoritmi\TSP\Documentazione\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Desktop\SUPSI\terza\2semestre\algoritmi\Progetto_twoopt\TSP\Documentazione\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2F582E9-D13E-496E-8FAA-A5B3510898BD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B16F1B1-4E98-4997-80F0-89AEA486CDD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{96F14A57-E4E0-4A00-8F7F-8B3688CEB5D0}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nome file</t>
   </si>
@@ -76,13 +76,16 @@
   </si>
   <si>
     <t>Media errori</t>
+  </si>
+  <si>
+    <t>SEED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +93,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -128,8 +138,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -152,17 +180,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -482,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A20ED122-453E-42A3-9FC5-925B21CF9992}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -494,10 +539,10 @@
     <col min="2" max="2" width="19.5546875" customWidth="1"/>
     <col min="3" max="3" width="22.21875" customWidth="1"/>
     <col min="4" max="4" width="14.33203125" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -510,8 +555,11 @@
       <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -519,14 +567,18 @@
         <v>6110</v>
       </c>
       <c r="C2" s="3">
-        <v>7028</v>
+        <v>6110</v>
       </c>
       <c r="D2" s="3">
         <f>((C2-B2)/C2)*100</f>
-        <v>13.062037564029596</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1553592951193</v>
+      </c>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -534,14 +586,18 @@
         <v>15780</v>
       </c>
       <c r="C3" s="3">
-        <v>17186</v>
+        <v>15781</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" ref="D3:D11" si="0">((C3-B3)/C3)*100</f>
-        <v>8.1810776213196785</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6.3367340472720362E-3</v>
+      </c>
+      <c r="E3" s="7">
+        <v>1553593210405</v>
+      </c>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -549,14 +605,18 @@
         <v>538</v>
       </c>
       <c r="C4" s="3">
-        <v>561</v>
+        <v>538</v>
       </c>
       <c r="D4" s="3">
         <f t="shared" si="0"/>
-        <v>4.0998217468805702</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>1553593570081</v>
+      </c>
+      <c r="F4" s="10"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -564,14 +624,18 @@
         <v>22249</v>
       </c>
       <c r="C5" s="3">
-        <v>24816</v>
+        <v>22869</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>10.344132817537073</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>2.7110936201845295</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1553793401381</v>
+      </c>
+      <c r="F5" s="11"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -579,14 +643,18 @@
         <v>21282</v>
       </c>
       <c r="C6" s="3">
-        <v>24200</v>
+        <v>21282</v>
       </c>
       <c r="D6" s="3">
         <f t="shared" si="0"/>
-        <v>12.057851239669422</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1553593959586</v>
+      </c>
+      <c r="F6" s="10"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -594,14 +662,18 @@
         <v>42029</v>
       </c>
       <c r="C7" s="3">
-        <v>49625</v>
+        <v>42029</v>
       </c>
       <c r="D7" s="3">
         <f t="shared" si="0"/>
-        <v>15.306801007556675</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+      <c r="E7" s="7">
+        <v>1553681533325</v>
+      </c>
+      <c r="F7" s="9"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -609,14 +681,17 @@
         <v>50778</v>
       </c>
       <c r="C8" s="3">
-        <v>54154</v>
+        <v>51105</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>6.2340731986556852</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.63985911358966829</v>
+      </c>
+      <c r="E8" s="7">
+        <v>1553707441798</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -624,14 +699,17 @@
         <v>107217</v>
       </c>
       <c r="C9" s="3">
-        <v>117612</v>
+        <v>107330</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>8.8383838383838391</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+        <v>0.10528277275691793</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1553595355487</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -639,14 +717,17 @@
         <v>8806</v>
       </c>
       <c r="C10" s="3">
-        <v>9610</v>
+        <v>9222</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>8.3662851196670136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+        <v>4.5109520711342448</v>
+      </c>
+      <c r="E10" s="7">
+        <v>1553723496331</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -654,20 +735,23 @@
         <v>224094</v>
       </c>
       <c r="C11" s="3">
-        <v>261388</v>
+        <v>231383</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>14.267678699863803</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>3.1501882160746466</v>
+      </c>
+      <c r="E11" s="7">
+        <v>1553610445037</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
         <v>14</v>
       </c>
       <c r="D12" s="5">
         <f>AVERAGE(D2:D11)</f>
-        <v>10.075814285356333</v>
+        <v>1.1123712527787277</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modifica per introduzione del test
</commit_message>
<xml_diff>
--- a/Documentazione/excel/calcolo_perc.xlsx
+++ b/Documentazione/excel/calcolo_perc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Desktop\SUPSI\terza\2semestre\algoritmi\Progetto_twoopt\TSP\Documentazione\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Desktop\TSP\Documentazione\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B16F1B1-4E98-4997-80F0-89AEA486CDD6}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E8D2F3-A4E9-4D8A-96DE-F2617EA61DC4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{96F14A57-E4E0-4A00-8F7F-8B3688CEB5D0}"/>
   </bookViews>
@@ -101,7 +101,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,18 +144,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -195,7 +183,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -205,9 +193,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="1" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -530,7 +516,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -574,7 +560,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="7">
-        <v>1553592951193</v>
+        <v>1556278594271</v>
       </c>
       <c r="F2" s="8"/>
     </row>
@@ -586,16 +572,16 @@
         <v>15780</v>
       </c>
       <c r="C3" s="3">
-        <v>15781</v>
+        <v>15780</v>
       </c>
       <c r="D3" s="3">
         <f t="shared" ref="D3:D11" si="0">((C3-B3)/C3)*100</f>
-        <v>6.3367340472720362E-3</v>
+        <v>0</v>
       </c>
       <c r="E3" s="7">
-        <v>1553593210405</v>
-      </c>
-      <c r="F3" s="9"/>
+        <v>1556281085299</v>
+      </c>
+      <c r="F3" s="8"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
@@ -612,9 +598,9 @@
         <v>0</v>
       </c>
       <c r="E4" s="7">
-        <v>1553593570081</v>
-      </c>
-      <c r="F4" s="10"/>
+        <v>1556289023497</v>
+      </c>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -624,16 +610,16 @@
         <v>22249</v>
       </c>
       <c r="C5" s="3">
-        <v>22869</v>
+        <v>22648</v>
       </c>
       <c r="D5" s="3">
         <f t="shared" si="0"/>
-        <v>2.7110936201845295</v>
+        <v>1.761744966442953</v>
       </c>
       <c r="E5" s="7">
-        <v>1553793401381</v>
-      </c>
-      <c r="F5" s="11"/>
+        <v>1556198455513</v>
+      </c>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -650,9 +636,9 @@
         <v>0</v>
       </c>
       <c r="E6" s="7">
-        <v>1553593959586</v>
-      </c>
-      <c r="F6" s="10"/>
+        <v>1556295011782</v>
+      </c>
+      <c r="F6" s="9"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
@@ -669,7 +655,7 @@
         <v>0</v>
       </c>
       <c r="E7" s="7">
-        <v>1553681533325</v>
+        <v>1556036354013</v>
       </c>
       <c r="F7" s="9"/>
     </row>
@@ -681,15 +667,16 @@
         <v>50778</v>
       </c>
       <c r="C8" s="3">
-        <v>51105</v>
+        <v>50923</v>
       </c>
       <c r="D8" s="3">
         <f t="shared" si="0"/>
-        <v>0.63985911358966829</v>
+        <v>0.28474363254325158</v>
       </c>
       <c r="E8" s="7">
-        <v>1553707441798</v>
-      </c>
+        <v>1556227370289</v>
+      </c>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
@@ -699,15 +686,16 @@
         <v>107217</v>
       </c>
       <c r="C9" s="3">
-        <v>107330</v>
+        <v>107217</v>
       </c>
       <c r="D9" s="3">
         <f t="shared" si="0"/>
-        <v>0.10528277275691793</v>
+        <v>0</v>
       </c>
       <c r="E9" s="7">
-        <v>1553595355487</v>
-      </c>
+        <v>1556214127505</v>
+      </c>
+      <c r="F9" s="8"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -717,15 +705,16 @@
         <v>8806</v>
       </c>
       <c r="C10" s="3">
-        <v>9222</v>
+        <v>9124</v>
       </c>
       <c r="D10" s="3">
         <f t="shared" si="0"/>
-        <v>4.5109520711342448</v>
+        <v>3.4853134590092067</v>
       </c>
       <c r="E10" s="7">
-        <v>1553723496331</v>
-      </c>
+        <v>1556388058827</v>
+      </c>
+      <c r="F10" s="8"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -735,15 +724,16 @@
         <v>224094</v>
       </c>
       <c r="C11" s="3">
-        <v>231383</v>
+        <v>226707</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>3.1501882160746466</v>
+        <v>1.1525890246000343</v>
       </c>
       <c r="E11" s="7">
-        <v>1553610445037</v>
-      </c>
+        <v>1556207871133</v>
+      </c>
+      <c r="F11" s="8"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="C12" s="4" t="s">
@@ -751,7 +741,7 @@
       </c>
       <c r="D12" s="5">
         <f>AVERAGE(D2:D11)</f>
-        <v>1.1123712527787277</v>
+        <v>0.66843910825954467</v>
       </c>
     </row>
   </sheetData>

</xml_diff>